<commit_message>
Add corrected Average, Calculate .1 Goal Seeker
</commit_message>
<xml_diff>
--- a/Data/Implied Volatility/Average.xlsx
+++ b/Data/Implied Volatility/Average.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Row Labels</t>
   </si>
@@ -83,14 +83,21 @@
   </si>
   <si>
     <t>Database Mean</t>
+  </si>
+  <si>
+    <t>Is this crazy number? &gt; 1</t>
+  </si>
+  <si>
+    <t>Solver - Only LNKD result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -129,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -143,10 +150,13 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -485,7 +495,7 @@
   <dimension ref="B1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +504,7 @@
     <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -632,14 +642,14 @@
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
+      <c r="C11" s="7">
+        <v>1.0133564799536847</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1.4005665966641001</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1.0133564799536849</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -698,7 +708,7 @@
         <v>0.26081768815256734</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
@@ -715,7 +725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>1</v>
       </c>
@@ -732,7 +742,7 @@
         <v>9.0277074250341593E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -749,7 +759,7 @@
         <v>6.0211816932207009E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
@@ -766,7 +776,7 @@
         <v>3.5862505422388576E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
@@ -786,7 +796,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
@@ -803,7 +813,7 @@
         <v>2.5375591021351264E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>6</v>
       </c>
@@ -820,7 +830,7 @@
         <v>2.0248504658209299E-3</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>7</v>
       </c>
@@ -837,7 +847,7 @@
         <v>7.2159109089093801E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>8</v>
       </c>
@@ -854,24 +864,30 @@
         <v>4.2729861775487779E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1424265188571565</v>
       </c>
       <c r="D26" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="4" t="e">
+        <v>0.18253259951331366</v>
+      </c>
+      <c r="E26" s="4">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.15977622761760896</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>10</v>
       </c>
@@ -888,7 +904,7 @@
         <v>1.9873028482435711E-3</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -905,7 +921,7 @@
         <v>0.10566452176458183</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>12</v>
       </c>
@@ -922,7 +938,7 @@
         <v>4.5531167271943902E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>16</v>
       </c>

</xml_diff>